<commit_message>
Add baseline for jordan network and results for no. 3 of elman keras
</commit_message>
<xml_diff>
--- a/projects.xlsx
+++ b/projects.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>Table 1</t>
   </si>
@@ -74,6 +74,9 @@
     <t>50</t>
   </si>
   <si>
+    <t xml:space="preserve"> 96.45/93.65</t>
+  </si>
+  <si>
     <t>25</t>
   </si>
   <si>
@@ -101,9 +104,15 @@
     <t>95.41/92.54</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>94.01/91.58</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>0.001</t>
   </si>
   <si>
@@ -120,6 +129,9 @@
   </si>
   <si>
     <t>200</t>
+  </si>
+  <si>
+    <t>95.64/92.22</t>
   </si>
   <si>
     <t>Since the learning rate was too low, we increase it again, but at the same time, we also increase the dimensionality for the embedding</t>
@@ -1990,7 +2002,9 @@
       <c r="J3" t="s" s="6">
         <v>19</v>
       </c>
-      <c r="K3" s="8"/>
+      <c r="K3" t="s" s="8">
+        <v>20</v>
+      </c>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
@@ -2030,13 +2044,13 @@
         <v>17</v>
       </c>
       <c r="J4" t="s" s="13">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K4" t="s" s="14">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L4" t="s" s="15">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
@@ -2243,7 +2257,7 @@
     </row>
     <row r="13" ht="43" customHeight="1">
       <c r="A13" t="s" s="24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s" s="25">
         <v>2</v>
@@ -2258,16 +2272,16 @@
         <v>8</v>
       </c>
       <c r="F13" t="s" s="26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s" s="26">
         <v>10</v>
       </c>
       <c r="H13" t="s" s="26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I13" t="s" s="27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J13" s="28"/>
       <c r="K13" s="29"/>
@@ -2289,7 +2303,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s" s="32">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s" s="32">
         <v>17</v>
@@ -2304,7 +2318,7 @@
         <v>19</v>
       </c>
       <c r="H14" t="s" s="33">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I14" s="34"/>
       <c r="J14" s="35"/>
@@ -2322,12 +2336,14 @@
       <c r="V14" s="35"/>
     </row>
     <row r="15" ht="51" customHeight="1">
-      <c r="A15" s="30"/>
+      <c r="A15" t="s" s="30">
+        <v>30</v>
+      </c>
       <c r="B15" t="s" s="36">
         <v>13</v>
       </c>
       <c r="C15" t="s" s="37">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s" s="37">
         <v>17</v>
@@ -2339,13 +2355,13 @@
         <v>17</v>
       </c>
       <c r="G15" t="s" s="37">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H15" t="s" s="38">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I15" t="s" s="11">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
@@ -2362,22 +2378,24 @@
       <c r="V15" s="16"/>
     </row>
     <row r="16" ht="36.65" customHeight="1">
-      <c r="A16" s="39"/>
+      <c r="A16" t="s" s="39">
+        <v>32</v>
+      </c>
       <c r="B16" s="40"/>
       <c r="C16" t="s" s="41">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="41"/>
       <c r="F16" s="41"/>
       <c r="G16" t="s" s="41">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H16" t="s" s="19">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I16" t="s" s="11">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
@@ -2394,24 +2412,28 @@
       <c r="V16" s="11"/>
     </row>
     <row r="17" ht="50.35" customHeight="1">
-      <c r="A17" s="39"/>
+      <c r="A17" t="s" s="39">
+        <v>13</v>
+      </c>
       <c r="B17" s="10"/>
       <c r="C17" t="s" s="11">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s" s="11">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" t="s" s="11">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G17" t="s" s="11">
-        <v>31</v>
-      </c>
-      <c r="H17" s="19"/>
+        <v>34</v>
+      </c>
+      <c r="H17" t="s" s="19">
+        <v>39</v>
+      </c>
       <c r="I17" t="s" s="11">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
@@ -2430,11 +2452,19 @@
     <row r="18" ht="22.35" customHeight="1">
       <c r="A18" s="39"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="C18" t="s" s="11">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s" s="11">
+        <v>38</v>
+      </c>
       <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="F18" t="s" s="11">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s" s="11">
+        <v>34</v>
+      </c>
       <c r="H18" s="19"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>

</xml_diff>